<commit_message>
i got how to push my file into the github
</commit_message>
<xml_diff>
--- a/feed.xlsx
+++ b/feed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{413B69EC-B53D-4574-9CDA-DE707616DF9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21F1ED0F-C597-4DFC-9E80-4753089CFF77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>4+7=11</t>
   </si>
@@ -33,13 +33,16 @@
     <t>lkdjflajljdlkfajlkjlfa</t>
   </si>
   <si>
-    <t>akjdhkjfhakhdkjfhaf</t>
-  </si>
-  <si>
     <t>kjdkhfhkahkdfhkhdkhfkjdhf</t>
   </si>
   <si>
     <t>adfadfadfaf</t>
+  </si>
+  <si>
+    <t>lljlkfljkajlfjlajf</t>
+  </si>
+  <si>
+    <t>2+3=5</t>
   </si>
 </sst>
 </file>
@@ -357,10 +360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -375,18 +378,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>2</v>
-      </c>
-    </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>